<commit_message>
manage student crud operation
</commit_message>
<xml_diff>
--- a/db_design.xlsx
+++ b/db_design.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work-Folder\JS-React-Node\practice-work\modulejs_oop-express-graphql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work-Folder\JS-React-Node\Projects\training-management_course-listing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860CD923-48FE-404D-8526-AD1B2405E211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190EACA9-64B5-4289-AA00-603B20622E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{A36513BB-FC7C-47B4-AA0C-19649E186ADF}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="77">
   <si>
     <t>Users Table</t>
   </si>
@@ -245,6 +244,18 @@
   </si>
   <si>
     <t>instructor 5</t>
+  </si>
+  <si>
+    <t>Api_accessed_user Table</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>api_key</t>
+  </si>
+  <si>
+    <t>…....</t>
   </si>
 </sst>
 </file>
@@ -392,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -415,26 +426,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -446,11 +445,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1010,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B92ACA-5C0B-4C8D-94FD-291C7F628D35}">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,29 +1029,30 @@
     <col min="6" max="6" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="K1" s="8" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="K1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1281,7 +1289,7 @@
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="11"/>
+      <c r="M8" s="8"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1306,7 +1314,7 @@
       <c r="H9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M9" s="12"/>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1318,16 +1326,16 @@
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1339,16 +1347,16 @@
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1360,16 +1368,16 @@
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1381,16 +1389,16 @@
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1402,73 +1410,74 @@
       <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-    </row>
-    <row r="15" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="D14" s="17"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-    </row>
-    <row r="16" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-    </row>
-    <row r="17" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="F19" s="8" t="s">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="E19" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="I19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="19"/>
-      <c r="K19" s="8" t="s">
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="M19" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="19"/>
-    </row>
-    <row r="20" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
@@ -1478,28 +1487,35 @@
       <c r="C20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="E20" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="F20" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="K20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="20"/>
-      <c r="K20" s="3" t="s">
+      <c r="M20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="N20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="O20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N20" s="20"/>
-    </row>
-    <row r="21" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1509,28 +1525,35 @@
       <c r="C21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="1">
+      <c r="E21" s="1">
         <v>1</v>
       </c>
+      <c r="F21" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="G21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="15"/>
-      <c r="K21" s="1">
+      <c r="K21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="5">
         <v>1</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="N21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N21" s="15"/>
-    </row>
-    <row r="22" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O21" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -1540,28 +1563,35 @@
       <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="1">
+      <c r="E22" s="1">
         <v>2</v>
       </c>
+      <c r="F22" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="G22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="5">
+        <v>2</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="15"/>
-      <c r="K22" s="1">
+      <c r="K22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" s="5">
         <v>2</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="N22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N22" s="15"/>
-    </row>
-    <row r="23" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O22" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -1571,28 +1601,35 @@
       <c r="C23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="1">
+      <c r="E23" s="1">
         <v>3</v>
       </c>
+      <c r="F23" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="5">
+        <v>3</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23" s="15"/>
-      <c r="K23" s="1">
+      <c r="K23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" s="5">
         <v>3</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="N23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N23" s="15"/>
-    </row>
-    <row r="24" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O23" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4</v>
       </c>
@@ -1602,28 +1639,29 @@
       <c r="C24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="1">
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="I24" s="5">
         <v>4</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="J24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I24" s="15"/>
-      <c r="K24" s="1">
+      <c r="K24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" s="5">
         <v>4</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="N24" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N24" s="15"/>
-    </row>
-    <row r="25" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O24" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>5</v>
       </c>
@@ -1633,28 +1671,29 @@
       <c r="C25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="1">
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="I25" s="5">
         <v>5</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="J25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I25" s="15"/>
-      <c r="K25" s="1">
+      <c r="K25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" s="5">
         <v>5</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="N25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N25" s="15"/>
-    </row>
-    <row r="26" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O25" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>6</v>
       </c>
@@ -1664,18 +1703,20 @@
       <c r="C26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="1">
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="I26" s="5">
         <v>6</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="J26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I26" s="15"/>
-    </row>
-    <row r="27" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>7</v>
       </c>
@@ -1685,342 +1726,288 @@
       <c r="C27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="1">
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="I27" s="5">
         <v>7</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="J27" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I27" s="15"/>
-    </row>
-    <row r="28" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>8</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>9</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>10</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>11</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="K27" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
+      <c r="E31" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="K31" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+    </row>
+    <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>1</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="5">
+        <v>1</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K33" s="5">
+        <v>1</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>2</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="5">
+        <v>2</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K34" s="5">
+        <v>2</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
+      <c r="A35" s="5">
+        <v>3</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="5">
+        <v>3</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K35" s="5">
+        <v>3</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
-      <c r="E36" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="K36" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-    </row>
-    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M37" s="3" t="s">
-        <v>43</v>
+      <c r="A36" s="5">
+        <v>4</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="5">
+        <v>4</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K36" s="5">
+        <v>4</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>5</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="5">
+        <v>5</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K37" s="5">
+        <v>5</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>49</v>
       </c>
       <c r="K38" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
-        <v>2</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="5">
-        <v>2</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K39" s="5">
-        <v>2</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="M39" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
-        <v>3</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="5">
-        <v>3</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K40" s="5">
-        <v>3</v>
-      </c>
-      <c r="L40" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
-        <v>4</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="5">
-        <v>4</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K41" s="5">
-        <v>4</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>5</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="5">
-        <v>5</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K42" s="5">
-        <v>5</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
-        <v>6</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="5">
-        <v>6</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K43" s="5">
-        <v>6</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="M43" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="K36:M36"/>
+  <mergeCells count="14">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="K1:N1"/>
-    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="E31:H31"/>
     <mergeCell ref="A15:N16"/>
     <mergeCell ref="D10:M14"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="K31:M31"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>